<commit_message>
Add annotations - Omar
</commit_message>
<xml_diff>
--- a/annotated_dataset/output_batch_3.xlsx
+++ b/annotated_dataset/output_batch_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathu\Desktop\Courses\4NL3\paraphrasing_detection\annotated_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\paraphrasing_detection\annotated_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1093905D-CE30-4D67-9600-08AF273FA8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E4C6A-36CF-4673-BE09-73F6680C25B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1261,20 +1261,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.3046875" customWidth="1"/>
-    <col min="2" max="2" width="36.921875" customWidth="1"/>
-    <col min="3" max="3" width="19.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.26953125" customWidth="1"/>
+    <col min="2" max="2" width="36.90625" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1301,13 +1301,15 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
       <c r="E2" s="2">
         <f>0.6*C2+0.4*D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1317,13 +1319,15 @@
       <c r="C3" s="2">
         <v>0.83333333333333326</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E66" si="0">0.6*C3+0.4*D3</f>
-        <v>0.49999999999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1333,13 +1337,15 @@
       <c r="C4" s="2">
         <v>0.6</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1349,13 +1355,15 @@
       <c r="C5" s="2">
         <v>0.75</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1365,13 +1373,15 @@
       <c r="C6" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1381,13 +1391,15 @@
       <c r="C7" s="2">
         <v>0.25</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1397,13 +1409,15 @@
       <c r="C8" s="2">
         <v>0.64393939393939392</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0.38636363636363635</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.58636363636363642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1413,13 +1427,15 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1429,13 +1445,15 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1445,13 +1463,15 @@
       <c r="C11" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.39999999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1461,13 +1481,15 @@
       <c r="C12" s="2">
         <v>0.375</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.22499999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1477,13 +1499,15 @@
       <c r="C13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1493,13 +1517,15 @@
       <c r="C14" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.39999999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -1509,13 +1535,15 @@
       <c r="C15" s="2">
         <v>0.73660714285714279</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.44196428571428564</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.64196428571428565</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1525,13 +1553,15 @@
       <c r="C16" s="2">
         <v>0.4642857142857143</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>0.27857142857142858</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.47857142857142859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -1541,13 +1571,15 @@
       <c r="C17" s="2">
         <v>0.53977272727272729</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
         <v>0.32386363636363635</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1557,13 +1589,15 @@
       <c r="C18" s="2">
         <v>0</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -1573,13 +1607,15 @@
       <c r="C19" s="2">
         <v>0.73888888888888893</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>0.44333333333333336</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.64333333333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1589,13 +1625,15 @@
       <c r="C20" s="2">
         <v>0.16666666666666671</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>0.10000000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
@@ -1605,13 +1643,15 @@
       <c r="C21" s="2">
         <v>0.54595588235294112</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>0.32757352941176465</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.72757352941176467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
@@ -1621,13 +1661,15 @@
       <c r="C22" s="2">
         <v>0.44285714285714278</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>0.26571428571428568</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
@@ -1637,13 +1679,15 @@
       <c r="C23" s="2">
         <v>0.4642857142857143</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>0.27857142857142858</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
@@ -1653,13 +1697,15 @@
       <c r="C24" s="2">
         <v>0.5</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
@@ -1669,13 +1715,15 @@
       <c r="C25" s="2">
         <v>0.4375</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E25" s="2">
         <f t="shared" si="0"/>
-        <v>0.26250000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.46250000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1685,13 +1733,15 @@
       <c r="C26" s="2">
         <v>0.79166666666666674</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
       <c r="E26" s="2">
         <f t="shared" si="0"/>
-        <v>0.47500000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1701,13 +1751,15 @@
       <c r="C27" s="2">
         <v>0.75213675213675213</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
       <c r="E27" s="2">
         <f t="shared" si="0"/>
-        <v>0.45128205128205123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.85128205128205126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -1717,13 +1769,15 @@
       <c r="C28" s="2">
         <v>0.89444444444444438</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
       <c r="E28" s="2">
         <f t="shared" si="0"/>
-        <v>0.53666666666666663</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.93666666666666665</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1733,13 +1787,15 @@
       <c r="C29" s="2">
         <v>0.66818181818181821</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
       <c r="E29" s="2">
         <f t="shared" si="0"/>
-        <v>0.40090909090909094</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.80090909090909101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1749,13 +1805,15 @@
       <c r="C30" s="2">
         <v>0.22222222222222221</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -1765,13 +1823,15 @@
       <c r="C31" s="2">
         <v>0.79370629370629375</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
       <c r="E31" s="2">
         <f t="shared" si="0"/>
-        <v>0.47622377622377621</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.87622377622377623</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -1781,13 +1841,15 @@
       <c r="C32" s="2">
         <v>0</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
       <c r="E32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1797,13 +1859,15 @@
       <c r="C33" s="2">
         <v>0.93541666666666667</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
       <c r="E33" s="2">
         <f t="shared" si="0"/>
-        <v>0.56125000000000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.96125000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -1813,13 +1877,15 @@
       <c r="C34" s="2">
         <v>1</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
       <c r="E34" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -1829,13 +1895,15 @@
       <c r="C35" s="2">
         <v>0.73888888888888893</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
       <c r="E35" s="2">
         <f t="shared" si="0"/>
-        <v>0.44333333333333336</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.84333333333333338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -1845,13 +1913,15 @@
       <c r="C36" s="2">
         <v>0.11805555555555559</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E36" s="2">
         <f t="shared" si="0"/>
-        <v>7.0833333333333359E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.27083333333333337</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -1861,13 +1931,15 @@
       <c r="C37" s="2">
         <v>0.5</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
       <c r="E37" s="2">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>76</v>
       </c>
@@ -1877,13 +1949,15 @@
       <c r="C38" s="2">
         <v>0</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E38" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>78</v>
       </c>
@@ -1893,13 +1967,15 @@
       <c r="C39" s="2">
         <v>0.50256410256410255</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
       <c r="E39" s="2">
         <f t="shared" si="0"/>
-        <v>0.30153846153846153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.70153846153846156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
@@ -1909,13 +1985,15 @@
       <c r="C40" s="2">
         <v>0.27083333333333331</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E40" s="2">
         <f t="shared" si="0"/>
-        <v>0.16249999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.36249999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
@@ -1925,13 +2003,15 @@
       <c r="C41" s="2">
         <v>0.75757575757575757</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E41" s="2">
         <f t="shared" si="0"/>
-        <v>0.45454545454545453</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.65454545454545454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
@@ -1941,13 +2021,15 @@
       <c r="C42" s="2">
         <v>0.50674662668665671</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
       <c r="E42" s="2">
         <f t="shared" si="0"/>
-        <v>0.30404797601199401</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.70404797601199398</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -1957,13 +2039,15 @@
       <c r="C43" s="2">
         <v>0</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
       <c r="E43" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="218.6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>88</v>
       </c>
@@ -1973,13 +2057,15 @@
       <c r="C44" s="2">
         <v>0.85803424092409242</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
       <c r="E44" s="2">
         <f t="shared" si="0"/>
-        <v>0.51482054455445547</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.91482054455445549</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
@@ -1989,13 +2075,15 @@
       <c r="C45" s="2">
         <v>0.73529411764705888</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
       <c r="E45" s="2">
         <f t="shared" si="0"/>
-        <v>0.44117647058823534</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.84117647058823541</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -2005,13 +2093,15 @@
       <c r="C46" s="2">
         <v>0.83333333333333326</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E46" s="2">
         <f t="shared" si="0"/>
-        <v>0.49999999999999994</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>94</v>
       </c>
@@ -2021,13 +2111,15 @@
       <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
       <c r="E47" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>96</v>
       </c>
@@ -2037,13 +2129,15 @@
       <c r="C48" s="2">
         <v>0.82499999999999996</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
       <c r="E48" s="2">
         <f t="shared" si="0"/>
-        <v>0.49499999999999994</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>98</v>
       </c>
@@ -2053,13 +2147,15 @@
       <c r="C49" s="2">
         <v>0.7525252525252526</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
       <c r="E49" s="2">
         <f t="shared" si="0"/>
-        <v>0.45151515151515154</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.85151515151515156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
@@ -2069,13 +2165,15 @@
       <c r="C50" s="2">
         <v>0.1130952380952381</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E50" s="2">
         <f t="shared" si="0"/>
-        <v>6.7857142857142852E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.26785714285714285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -2085,13 +2183,15 @@
       <c r="C51" s="2">
         <v>0.64645308924485123</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
       <c r="E51" s="2">
         <f t="shared" si="0"/>
-        <v>0.38787185354691073</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.78787185354691069</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2101,13 +2201,15 @@
       <c r="C52" s="2">
         <v>0</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
       <c r="E52" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>106</v>
       </c>
@@ -2117,13 +2219,15 @@
       <c r="C53" s="2">
         <v>1</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
       <c r="E53" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
@@ -2133,13 +2237,15 @@
       <c r="C54" s="2">
         <v>0.7525252525252526</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E54" s="2">
         <f t="shared" si="0"/>
-        <v>0.45151515151515154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.6515151515151516</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -2149,13 +2255,15 @@
       <c r="C55" s="2">
         <v>0.87121212121212122</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
       <c r="E55" s="2">
         <f t="shared" si="0"/>
-        <v>0.52272727272727271</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.92272727272727273</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2165,13 +2273,15 @@
       <c r="C56" s="2">
         <v>0</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
       <c r="E56" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>114</v>
       </c>
@@ -2181,13 +2291,15 @@
       <c r="C57" s="2">
         <v>0.65625</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
       <c r="E57" s="2">
         <f t="shared" si="0"/>
-        <v>0.39374999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.79374999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>116</v>
       </c>
@@ -2197,13 +2309,15 @@
       <c r="C58" s="2">
         <v>0.51249999999999996</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E58" s="2">
         <f t="shared" si="0"/>
-        <v>0.30749999999999994</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.50749999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>118</v>
       </c>
@@ -2213,13 +2327,15 @@
       <c r="C59" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
       <c r="E59" s="2">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>120</v>
       </c>
@@ -2229,13 +2345,15 @@
       <c r="C60" s="2">
         <v>0.6</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
       <c r="E60" s="2">
         <f t="shared" si="0"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>122</v>
       </c>
@@ -2245,13 +2363,15 @@
       <c r="C61" s="2">
         <v>0.7142857142857143</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
       <c r="E61" s="2">
         <f t="shared" si="0"/>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.82857142857142851</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>124</v>
       </c>
@@ -2261,13 +2381,15 @@
       <c r="C62" s="2">
         <v>0.38181818181818178</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
       <c r="E62" s="2">
         <f t="shared" si="0"/>
-        <v>0.22909090909090907</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.62909090909090915</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>126</v>
       </c>
@@ -2277,13 +2399,15 @@
       <c r="C63" s="2">
         <v>0</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E63" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>128</v>
       </c>
@@ -2293,13 +2417,15 @@
       <c r="C64" s="2">
         <v>1</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
       <c r="E64" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>129</v>
       </c>
@@ -2309,13 +2435,15 @@
       <c r="C65" s="2">
         <v>1</v>
       </c>
-      <c r="D65" s="2"/>
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
       <c r="E65" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>131</v>
       </c>
@@ -2325,13 +2453,15 @@
       <c r="C66" s="2">
         <v>0.73907563025210088</v>
       </c>
-      <c r="D66" s="2"/>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
       <c r="E66" s="2">
         <f t="shared" si="0"/>
-        <v>0.44344537815126051</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.84344537815126053</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>133</v>
       </c>
@@ -2341,13 +2471,15 @@
       <c r="C67" s="2">
         <v>0.5410256410256411</v>
       </c>
-      <c r="D67" s="2"/>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
       <c r="E67" s="2">
         <f t="shared" ref="E67:E130" si="1">0.6*C67+0.4*D67</f>
-        <v>0.32461538461538464</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.72461538461538466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>135</v>
       </c>
@@ -2357,13 +2489,15 @@
       <c r="C68" s="2">
         <v>0</v>
       </c>
-      <c r="D68" s="2"/>
+      <c r="D68" s="2">
+        <v>0</v>
+      </c>
       <c r="E68" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>137</v>
       </c>
@@ -2373,13 +2507,15 @@
       <c r="C69" s="2">
         <v>0</v>
       </c>
-      <c r="D69" s="2"/>
+      <c r="D69" s="2">
+        <v>0</v>
+      </c>
       <c r="E69" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>139</v>
       </c>
@@ -2389,13 +2525,15 @@
       <c r="C70" s="2">
         <v>0.51428571428571423</v>
       </c>
-      <c r="D70" s="2"/>
+      <c r="D70" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E70" s="2">
         <f t="shared" si="1"/>
-        <v>0.30857142857142855</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.50857142857142856</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>141</v>
       </c>
@@ -2405,13 +2543,15 @@
       <c r="C71" s="2">
         <v>0.79285714285714293</v>
       </c>
-      <c r="D71" s="2"/>
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
       <c r="E71" s="2">
         <f t="shared" si="1"/>
-        <v>0.47571428571428576</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.87571428571428578</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
@@ -2421,13 +2561,15 @@
       <c r="C72" s="2">
         <v>0.65</v>
       </c>
-      <c r="D72" s="2"/>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
       <c r="E72" s="2">
         <f t="shared" si="1"/>
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>145</v>
       </c>
@@ -2437,13 +2579,15 @@
       <c r="C73" s="2">
         <v>0.75</v>
       </c>
-      <c r="D73" s="2"/>
+      <c r="D73" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E73" s="2">
         <f t="shared" si="1"/>
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.64999999999999991</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>147</v>
       </c>
@@ -2453,13 +2597,15 @@
       <c r="C74" s="2">
         <v>0.18333333333333329</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="D74" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E74" s="2">
         <f t="shared" si="1"/>
-        <v>0.10999999999999997</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>149</v>
       </c>
@@ -2469,13 +2615,15 @@
       <c r="C75" s="2">
         <v>0.54761904761904756</v>
       </c>
-      <c r="D75" s="2"/>
+      <c r="D75" s="2">
+        <v>1</v>
+      </c>
       <c r="E75" s="2">
         <f t="shared" si="1"/>
-        <v>0.32857142857142851</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.72857142857142854</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>151</v>
       </c>
@@ -2485,13 +2633,15 @@
       <c r="C76" s="2">
         <v>0.58441558441558439</v>
       </c>
-      <c r="D76" s="2"/>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
       <c r="E76" s="2">
         <f t="shared" si="1"/>
-        <v>0.3506493506493506</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.75064935064935057</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>153</v>
       </c>
@@ -2501,13 +2651,15 @@
       <c r="C77" s="2">
         <v>0.40584415584415579</v>
       </c>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="E77" s="2">
         <f t="shared" si="1"/>
-        <v>0.24350649350649345</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.64350649350649347</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>155</v>
       </c>
@@ -2517,13 +2669,15 @@
       <c r="C78" s="2">
         <v>0.67500000000000004</v>
       </c>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E78" s="2">
         <f t="shared" si="1"/>
-        <v>0.40500000000000003</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>157</v>
       </c>
@@ -2533,13 +2687,15 @@
       <c r="C79" s="2">
         <v>1</v>
       </c>
-      <c r="D79" s="2"/>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
       <c r="E79" s="2">
         <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>159</v>
       </c>
@@ -2549,13 +2705,15 @@
       <c r="C80" s="2">
         <v>0.48798076923076922</v>
       </c>
-      <c r="D80" s="2"/>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
       <c r="E80" s="2">
         <f t="shared" si="1"/>
-        <v>0.2927884615384615</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.69278846153846152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>161</v>
       </c>
@@ -2565,13 +2723,15 @@
       <c r="C81" s="2">
         <v>0.87884615384615383</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
       <c r="E81" s="2">
         <f t="shared" si="1"/>
-        <v>0.52730769230769226</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.92730769230769228</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>163</v>
       </c>
@@ -2581,13 +2741,15 @@
       <c r="C82" s="2">
         <v>0.75</v>
       </c>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
       <c r="E82" s="2">
         <f t="shared" si="1"/>
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>165</v>
       </c>
@@ -2597,13 +2759,15 @@
       <c r="C83" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D83" s="2"/>
+      <c r="D83" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E83" s="2">
         <f t="shared" si="1"/>
-        <v>0.39999999999999997</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>167</v>
       </c>
@@ -2613,13 +2777,15 @@
       <c r="C84" s="2">
         <v>0.77257004496713932</v>
       </c>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
       <c r="E84" s="2">
         <f t="shared" si="1"/>
-        <v>0.46354202698028357</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.86354202698028359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>169</v>
       </c>
@@ -2629,13 +2795,15 @@
       <c r="C85" s="2">
         <v>0.39285714285714279</v>
       </c>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
       <c r="E85" s="2">
         <f t="shared" si="1"/>
-        <v>0.23571428571428565</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.63571428571428568</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>171</v>
       </c>
@@ -2645,13 +2813,15 @@
       <c r="C86" s="2">
         <v>0.57427055702917773</v>
       </c>
-      <c r="D86" s="2"/>
+      <c r="D86" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E86" s="2">
         <f t="shared" si="1"/>
-        <v>0.34456233421750665</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.54456233421750666</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>173</v>
       </c>
@@ -2661,13 +2831,15 @@
       <c r="C87" s="2">
         <v>0</v>
       </c>
-      <c r="D87" s="2"/>
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
       <c r="E87" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>175</v>
       </c>
@@ -2677,13 +2849,15 @@
       <c r="C88" s="2">
         <v>0.89311594202898548</v>
       </c>
-      <c r="D88" s="2"/>
+      <c r="D88" s="2">
+        <v>1</v>
+      </c>
       <c r="E88" s="2">
         <f t="shared" si="1"/>
-        <v>0.53586956521739126</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
+        <v>0.93586956521739129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>177</v>
       </c>
@@ -2693,13 +2867,15 @@
       <c r="C89" s="2">
         <v>0.73642699926632427</v>
       </c>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
       <c r="E89" s="2">
         <f t="shared" si="1"/>
-        <v>0.44185619955979455</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.84185619955979463</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>179</v>
       </c>
@@ -2709,13 +2885,15 @@
       <c r="C90" s="2">
         <v>1</v>
       </c>
-      <c r="D90" s="2"/>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
       <c r="E90" s="2">
         <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>180</v>
       </c>
@@ -2725,13 +2903,15 @@
       <c r="C91" s="2">
         <v>0.47222222222222221</v>
       </c>
-      <c r="D91" s="2"/>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
       <c r="E91" s="2">
         <f t="shared" si="1"/>
-        <v>0.28333333333333333</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>182</v>
       </c>
@@ -2741,13 +2921,15 @@
       <c r="C92" s="2">
         <v>0</v>
       </c>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
       <c r="E92" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>184</v>
       </c>
@@ -2757,13 +2939,15 @@
       <c r="C93" s="2">
         <v>0</v>
       </c>
-      <c r="D93" s="2"/>
+      <c r="D93" s="2">
+        <v>0</v>
+      </c>
       <c r="E93" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>186</v>
       </c>
@@ -2773,13 +2957,15 @@
       <c r="C94" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
       <c r="E94" s="2">
         <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>188</v>
       </c>
@@ -2789,13 +2975,15 @@
       <c r="C95" s="2">
         <v>0.72727272727272729</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
       <c r="E95" s="2">
         <f t="shared" si="1"/>
-        <v>0.43636363636363634</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.83636363636363642</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>190</v>
       </c>
@@ -2805,13 +2993,15 @@
       <c r="C96" s="2">
         <v>0.10096153846153851</v>
       </c>
-      <c r="D96" s="2"/>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
       <c r="E96" s="2">
         <f t="shared" si="1"/>
         <v>6.0576923076923098E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>192</v>
       </c>
@@ -2821,13 +3011,15 @@
       <c r="C97" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D97" s="2"/>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
       <c r="E97" s="2">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>194</v>
       </c>
@@ -2837,13 +3029,15 @@
       <c r="C98" s="2">
         <v>0.76363636363636367</v>
       </c>
-      <c r="D98" s="2"/>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
       <c r="E98" s="2">
         <f t="shared" si="1"/>
-        <v>0.45818181818181819</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.85818181818181816</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>196</v>
       </c>
@@ -2853,13 +3047,15 @@
       <c r="C99" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D99" s="2"/>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
       <c r="E99" s="2">
         <f t="shared" si="1"/>
-        <v>0.19999999999999998</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>198</v>
       </c>
@@ -2869,13 +3065,15 @@
       <c r="C100" s="2">
         <v>0.95454545454545459</v>
       </c>
-      <c r="D100" s="2"/>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
       <c r="E100" s="2">
         <f t="shared" si="1"/>
-        <v>0.57272727272727275</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.97272727272727277</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>200</v>
       </c>
@@ -2885,13 +3083,15 @@
       <c r="C101" s="2">
         <v>0</v>
       </c>
-      <c r="D101" s="2"/>
+      <c r="D101" s="2">
+        <v>0</v>
+      </c>
       <c r="E101" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>202</v>
       </c>
@@ -2901,13 +3101,15 @@
       <c r="C102" s="2">
         <v>0.15476190476190479</v>
       </c>
-      <c r="D102" s="2"/>
+      <c r="D102" s="2">
+        <v>1</v>
+      </c>
       <c r="E102" s="2">
         <f t="shared" si="1"/>
-        <v>9.2857142857142874E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.49285714285714288</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>204</v>
       </c>
@@ -2917,13 +3119,15 @@
       <c r="C103" s="2">
         <v>0.30555555555555558</v>
       </c>
-      <c r="D103" s="2"/>
+      <c r="D103" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E103" s="2">
         <f t="shared" si="1"/>
-        <v>0.18333333333333335</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.38333333333333336</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>206</v>
       </c>
@@ -2933,13 +3137,15 @@
       <c r="C104" s="2">
         <v>0.86974789915966388</v>
       </c>
-      <c r="D104" s="2"/>
+      <c r="D104" s="2">
+        <v>1</v>
+      </c>
       <c r="E104" s="2">
         <f t="shared" si="1"/>
-        <v>0.52184873949579835</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.92184873949579837</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>208</v>
       </c>
@@ -2949,13 +3155,15 @@
       <c r="C105" s="2">
         <v>1</v>
       </c>
-      <c r="D105" s="2"/>
+      <c r="D105" s="2">
+        <v>1</v>
+      </c>
       <c r="E105" s="2">
         <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>210</v>
       </c>
@@ -2965,13 +3173,15 @@
       <c r="C106" s="2">
         <v>0.6004784688995215</v>
       </c>
-      <c r="D106" s="2"/>
+      <c r="D106" s="2">
+        <v>1</v>
+      </c>
       <c r="E106" s="2">
         <f t="shared" si="1"/>
-        <v>0.36028708133971288</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.7602870813397129</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>212</v>
       </c>
@@ -2981,13 +3191,15 @@
       <c r="C107" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D107" s="2"/>
+      <c r="D107" s="2">
+        <v>1</v>
+      </c>
       <c r="E107" s="2">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>214</v>
       </c>
@@ -2997,13 +3209,15 @@
       <c r="C108" s="2">
         <v>0.91097308488612838</v>
       </c>
-      <c r="D108" s="2"/>
+      <c r="D108" s="2">
+        <v>1</v>
+      </c>
       <c r="E108" s="2">
         <f t="shared" si="1"/>
-        <v>0.54658385093167705</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.94658385093167707</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>216</v>
       </c>
@@ -3013,13 +3227,15 @@
       <c r="C109" s="2">
         <v>0</v>
       </c>
-      <c r="D109" s="2"/>
+      <c r="D109" s="2">
+        <v>0</v>
+      </c>
       <c r="E109" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>218</v>
       </c>
@@ -3029,13 +3245,15 @@
       <c r="C110" s="2">
         <v>0.45</v>
       </c>
-      <c r="D110" s="2"/>
+      <c r="D110" s="2">
+        <v>1</v>
+      </c>
       <c r="E110" s="2">
         <f t="shared" si="1"/>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>220</v>
       </c>
@@ -3045,13 +3263,15 @@
       <c r="C111" s="2">
         <v>0.8035714285714286</v>
       </c>
-      <c r="D111" s="2"/>
+      <c r="D111" s="2">
+        <v>1</v>
+      </c>
       <c r="E111" s="2">
         <f t="shared" si="1"/>
-        <v>0.48214285714285715</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.88214285714285712</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>222</v>
       </c>
@@ -3061,13 +3281,15 @@
       <c r="C112" s="2">
         <v>0.64393939393939392</v>
       </c>
-      <c r="D112" s="2"/>
+      <c r="D112" s="2">
+        <v>1</v>
+      </c>
       <c r="E112" s="2">
         <f t="shared" si="1"/>
-        <v>0.38636363636363635</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.78636363636363638</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>224</v>
       </c>
@@ -3077,13 +3299,15 @@
       <c r="C113" s="2">
         <v>0.5892857142857143</v>
       </c>
-      <c r="D113" s="2"/>
+      <c r="D113" s="2">
+        <v>1</v>
+      </c>
       <c r="E113" s="2">
         <f t="shared" si="1"/>
-        <v>0.35357142857142859</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.75357142857142856</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>226</v>
       </c>
@@ -3093,13 +3317,15 @@
       <c r="C114" s="2">
         <v>0.5</v>
       </c>
-      <c r="D114" s="2"/>
+      <c r="D114" s="2">
+        <v>0</v>
+      </c>
       <c r="E114" s="2">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>228</v>
       </c>
@@ -3109,13 +3335,15 @@
       <c r="C115" s="2">
         <v>0.70138888888888884</v>
       </c>
-      <c r="D115" s="2"/>
+      <c r="D115" s="2">
+        <v>1</v>
+      </c>
       <c r="E115" s="2">
         <f t="shared" si="1"/>
-        <v>0.42083333333333328</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.8208333333333333</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>230</v>
       </c>
@@ -3125,13 +3353,15 @@
       <c r="C116" s="2">
         <v>0.1254901960784314</v>
       </c>
-      <c r="D116" s="2"/>
+      <c r="D116" s="2">
+        <v>0</v>
+      </c>
       <c r="E116" s="2">
         <f t="shared" si="1"/>
         <v>7.5294117647058831E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>232</v>
       </c>
@@ -3141,13 +3371,15 @@
       <c r="C117" s="2">
         <v>0.53333333333333333</v>
       </c>
-      <c r="D117" s="2"/>
+      <c r="D117" s="2">
+        <v>1</v>
+      </c>
       <c r="E117" s="2">
         <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>234</v>
       </c>
@@ -3157,13 +3389,15 @@
       <c r="C118" s="2">
         <v>0.42222222222222222</v>
       </c>
-      <c r="D118" s="2"/>
+      <c r="D118" s="2">
+        <v>1</v>
+      </c>
       <c r="E118" s="2">
         <f t="shared" si="1"/>
-        <v>0.2533333333333333</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
+        <v>0.65333333333333332</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>236</v>
       </c>
@@ -3173,13 +3407,15 @@
       <c r="C119" s="2">
         <v>0.532258064516129</v>
       </c>
-      <c r="D119" s="2"/>
+      <c r="D119" s="2">
+        <v>1</v>
+      </c>
       <c r="E119" s="2">
         <f t="shared" si="1"/>
-        <v>0.3193548387096774</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>0.71935483870967742</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>238</v>
       </c>
@@ -3189,13 +3425,15 @@
       <c r="C120" s="2">
         <v>0.70833333333333326</v>
       </c>
-      <c r="D120" s="2"/>
+      <c r="D120" s="2">
+        <v>1</v>
+      </c>
       <c r="E120" s="2">
         <f t="shared" si="1"/>
-        <v>0.42499999999999993</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>240</v>
       </c>
@@ -3205,13 +3443,15 @@
       <c r="C121" s="2">
         <v>0.5</v>
       </c>
-      <c r="D121" s="2"/>
+      <c r="D121" s="2">
+        <v>1</v>
+      </c>
       <c r="E121" s="2">
         <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>242</v>
       </c>
@@ -3221,13 +3461,15 @@
       <c r="C122" s="2">
         <v>0</v>
       </c>
-      <c r="D122" s="2"/>
+      <c r="D122" s="2">
+        <v>0</v>
+      </c>
       <c r="E122" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="247.75" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>244</v>
       </c>
@@ -3237,13 +3479,15 @@
       <c r="C123" s="2">
         <v>0</v>
       </c>
-      <c r="D123" s="2"/>
+      <c r="D123" s="2">
+        <v>0</v>
+      </c>
       <c r="E123" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>246</v>
       </c>
@@ -3253,13 +3497,15 @@
       <c r="C124" s="2">
         <v>0.58333333333333326</v>
       </c>
-      <c r="D124" s="2"/>
+      <c r="D124" s="2">
+        <v>1</v>
+      </c>
       <c r="E124" s="2">
         <f t="shared" si="1"/>
-        <v>0.34999999999999992</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>248</v>
       </c>
@@ -3269,13 +3515,15 @@
       <c r="C125" s="2">
         <v>1</v>
       </c>
-      <c r="D125" s="2"/>
+      <c r="D125" s="2">
+        <v>1</v>
+      </c>
       <c r="E125" s="2">
         <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>250</v>
       </c>
@@ -3285,13 +3533,15 @@
       <c r="C126" s="2">
         <v>0.88888888888888884</v>
       </c>
-      <c r="D126" s="2"/>
+      <c r="D126" s="2">
+        <v>1</v>
+      </c>
       <c r="E126" s="2">
         <f t="shared" si="1"/>
-        <v>0.53333333333333333</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>252</v>
       </c>
@@ -3301,13 +3551,15 @@
       <c r="C127" s="2">
         <v>0.83333333333333326</v>
       </c>
-      <c r="D127" s="2"/>
+      <c r="D127" s="2">
+        <v>1</v>
+      </c>
       <c r="E127" s="2">
         <f t="shared" si="1"/>
-        <v>0.49999999999999994</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>254</v>
       </c>
@@ -3317,13 +3569,15 @@
       <c r="C128" s="2">
         <v>0</v>
       </c>
-      <c r="D128" s="2"/>
+      <c r="D128" s="2">
+        <v>0</v>
+      </c>
       <c r="E128" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>256</v>
       </c>
@@ -3333,13 +3587,15 @@
       <c r="C129" s="2">
         <v>0</v>
       </c>
-      <c r="D129" s="2"/>
+      <c r="D129" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E129" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>258</v>
       </c>
@@ -3349,13 +3605,15 @@
       <c r="C130" s="2">
         <v>0.9</v>
       </c>
-      <c r="D130" s="2"/>
+      <c r="D130" s="2">
+        <v>1</v>
+      </c>
       <c r="E130" s="2">
         <f t="shared" si="1"/>
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.94000000000000006</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>260</v>
       </c>
@@ -3365,13 +3623,15 @@
       <c r="C131" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D131" s="2"/>
+      <c r="D131" s="2">
+        <v>1</v>
+      </c>
       <c r="E131" s="2">
         <f t="shared" ref="E131:E146" si="2">0.6*C131+0.4*D131</f>
-        <v>0.39999999999999997</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>262</v>
       </c>
@@ -3381,13 +3641,15 @@
       <c r="C132" s="2">
         <v>0.45</v>
       </c>
-      <c r="D132" s="2"/>
+      <c r="D132" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E132" s="2">
         <f t="shared" si="2"/>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.47000000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>264</v>
       </c>
@@ -3397,13 +3659,15 @@
       <c r="C133" s="2">
         <v>0.47222222222222221</v>
       </c>
-      <c r="D133" s="2"/>
+      <c r="D133" s="2">
+        <v>1</v>
+      </c>
       <c r="E133" s="2">
         <f t="shared" si="2"/>
-        <v>0.28333333333333333</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>266</v>
       </c>
@@ -3413,13 +3677,15 @@
       <c r="C134" s="2">
         <v>0.26785714285714279</v>
       </c>
-      <c r="D134" s="2"/>
+      <c r="D134" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E134" s="2">
         <f t="shared" si="2"/>
-        <v>0.16071428571428567</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.36071428571428565</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>268</v>
       </c>
@@ -3429,13 +3695,15 @@
       <c r="C135" s="2">
         <v>0.25</v>
       </c>
-      <c r="D135" s="2"/>
+      <c r="D135" s="2">
+        <v>1</v>
+      </c>
       <c r="E135" s="2">
         <f t="shared" si="2"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>270</v>
       </c>
@@ -3445,13 +3713,15 @@
       <c r="C136" s="2">
         <v>0.70833333333333326</v>
       </c>
-      <c r="D136" s="2"/>
+      <c r="D136" s="2">
+        <v>1</v>
+      </c>
       <c r="E136" s="2">
         <f t="shared" si="2"/>
-        <v>0.42499999999999993</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>272</v>
       </c>
@@ -3461,13 +3731,15 @@
       <c r="C137" s="2">
         <v>0.18333333333333329</v>
       </c>
-      <c r="D137" s="2"/>
+      <c r="D137" s="2">
+        <v>0</v>
+      </c>
       <c r="E137" s="2">
         <f t="shared" si="2"/>
         <v>0.10999999999999997</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>274</v>
       </c>
@@ -3477,13 +3749,15 @@
       <c r="C138" s="2">
         <v>0.87301587301587302</v>
       </c>
-      <c r="D138" s="2"/>
+      <c r="D138" s="2">
+        <v>1</v>
+      </c>
       <c r="E138" s="2">
         <f t="shared" si="2"/>
-        <v>0.52380952380952384</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.92380952380952386</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>276</v>
       </c>
@@ -3493,13 +3767,15 @@
       <c r="C139" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D139" s="2"/>
+      <c r="D139" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E139" s="2">
         <f t="shared" si="2"/>
-        <v>0.39999999999999997</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>278</v>
       </c>
@@ -3509,13 +3785,15 @@
       <c r="C140" s="2">
         <v>0.67500000000000004</v>
       </c>
-      <c r="D140" s="2"/>
+      <c r="D140" s="2">
+        <v>1</v>
+      </c>
       <c r="E140" s="2">
         <f t="shared" si="2"/>
-        <v>0.40500000000000003</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>280</v>
       </c>
@@ -3525,13 +3803,15 @@
       <c r="C141" s="2">
         <v>0.70055413469735717</v>
       </c>
-      <c r="D141" s="2"/>
+      <c r="D141" s="2">
+        <v>1</v>
+      </c>
       <c r="E141" s="2">
         <f t="shared" si="2"/>
-        <v>0.42033248081841429</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.82033248081841426</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>282</v>
       </c>
@@ -3541,13 +3821,15 @@
       <c r="C142" s="2">
         <v>0.58333333333333326</v>
       </c>
-      <c r="D142" s="2"/>
+      <c r="D142" s="2">
+        <v>1</v>
+      </c>
       <c r="E142" s="2">
         <f t="shared" si="2"/>
-        <v>0.34999999999999992</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>284</v>
       </c>
@@ -3557,13 +3839,15 @@
       <c r="C143" s="2">
         <v>0.86205073995771664</v>
       </c>
-      <c r="D143" s="2"/>
+      <c r="D143" s="2">
+        <v>1</v>
+      </c>
       <c r="E143" s="2">
         <f t="shared" si="2"/>
-        <v>0.51723044397462992</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+        <v>0.91723044397462994</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>286</v>
       </c>
@@ -3573,13 +3857,15 @@
       <c r="C144" s="2">
         <v>0.36375661375661372</v>
       </c>
-      <c r="D144" s="2"/>
+      <c r="D144" s="2">
+        <v>1</v>
+      </c>
       <c r="E144" s="2">
         <f t="shared" si="2"/>
-        <v>0.21825396825396823</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.4">
+        <v>0.61825396825396828</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>288</v>
       </c>
@@ -3589,13 +3875,15 @@
       <c r="C145" s="2">
         <v>1</v>
       </c>
-      <c r="D145" s="2"/>
+      <c r="D145" s="2">
+        <v>1</v>
+      </c>
       <c r="E145" s="2">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>289</v>
       </c>
@@ -3605,10 +3893,12 @@
       <c r="C146" s="2">
         <v>0</v>
       </c>
-      <c r="D146" s="2"/>
+      <c r="D146" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E146" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>